<commit_message>
Updated backlog with more probable dates
</commit_message>
<xml_diff>
--- a/meetings/standups/Product Backlog Project Network Security Analysis Cloud Network.xlsx
+++ b/meetings/standups/Product Backlog Project Network Security Analysis Cloud Network.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="202300"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E02CFF8-BFF0-4D0B-8ED4-E9E69C01A6A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{415450CB-5CC5-4113-A6E5-BAF9D5F97AA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{D772D2C9-32D6-40F8-B3B7-1BC774CEBB4D}"/>
   </bookViews>
@@ -849,6 +849,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -873,9 +915,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -884,45 +923,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="15" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1276,7 +1276,7 @@
     <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
       <pane ySplit="12" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B2" sqref="B2"/>
-      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomLeft" activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1296,12 +1296,12 @@
       <c r="C2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
     </row>
     <row r="3" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C3" s="3" t="s">
@@ -1321,7 +1321,7 @@
       </c>
     </row>
     <row r="4" spans="3:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="C4" s="40" t="s">
+      <c r="C4" s="32" t="s">
         <v>17</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -1330,15 +1330,15 @@
       <c r="E4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="44">
-        <v>46050</v>
-      </c>
-      <c r="G4" s="44">
-        <v>46055</v>
+      <c r="F4" s="33">
+        <v>46050</v>
+      </c>
+      <c r="G4" s="33">
+        <v>46057</v>
       </c>
     </row>
     <row r="5" spans="3:10" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C5" s="40" t="s">
+      <c r="C5" s="32" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -1349,7 +1349,7 @@
       </c>
     </row>
     <row r="6" spans="3:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C6" s="40" t="s">
+      <c r="C6" s="32" t="s">
         <v>20</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -1378,7 +1378,7 @@
       <c r="H7" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="I7" s="50" t="s">
+      <c r="I7" s="39" t="s">
         <v>62</v>
       </c>
       <c r="J7" s="9" t="s">
@@ -1386,7 +1386,7 @@
       </c>
     </row>
     <row r="8" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C8" s="41" t="s">
+      <c r="C8" s="54" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="5"/>
@@ -1400,7 +1400,7 @@
       <c r="H8" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="I8" s="51" t="s">
+      <c r="I8" s="40" t="s">
         <v>65</v>
       </c>
       <c r="J8" s="11">
@@ -1408,7 +1408,7 @@
       </c>
     </row>
     <row r="9" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C9" s="42"/>
+      <c r="C9" s="55"/>
       <c r="D9" s="5" t="s">
         <v>52</v>
       </c>
@@ -1422,13 +1422,13 @@
       <c r="H9" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="I9" s="51"/>
+      <c r="I9" s="40"/>
       <c r="J9" s="11">
         <v>46043</v>
       </c>
     </row>
     <row r="10" spans="3:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="C10" s="43"/>
+      <c r="C10" s="56"/>
       <c r="D10" s="5" t="s">
         <v>24</v>
       </c>
@@ -1442,7 +1442,7 @@
       <c r="H10" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="I10" s="51" t="s">
+      <c r="I10" s="40" t="s">
         <v>64</v>
       </c>
       <c r="J10" s="11">
@@ -1466,7 +1466,7 @@
       <c r="H11" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="I11" s="51" t="s">
+      <c r="I11" s="40" t="s">
         <v>53</v>
       </c>
       <c r="J11" s="11"/>
@@ -1486,7 +1486,7 @@
       <c r="H12" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="I12" s="51" t="s">
+      <c r="I12" s="40" t="s">
         <v>63</v>
       </c>
       <c r="J12" s="11">
@@ -1494,7 +1494,7 @@
       </c>
     </row>
     <row r="13" spans="3:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="C13" s="56" t="s">
+      <c r="C13" s="45" t="s">
         <v>66</v>
       </c>
       <c r="D13" s="5"/>
@@ -1506,28 +1506,28 @@
         <v>46051</v>
       </c>
       <c r="H13" s="5"/>
-      <c r="I13" s="51"/>
+      <c r="I13" s="40"/>
       <c r="J13" s="11"/>
     </row>
     <row r="14" spans="3:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="C14" s="45" t="s">
+      <c r="C14" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="49" t="s">
+      <c r="D14" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="E14" s="46" t="s">
+      <c r="E14" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="F14" s="47"/>
-      <c r="G14" s="47">
+      <c r="F14" s="36"/>
+      <c r="G14" s="36">
         <v>46051</v>
       </c>
-      <c r="H14" s="46" t="s">
+      <c r="H14" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="I14" s="52"/>
-      <c r="J14" s="48"/>
+      <c r="I14" s="41"/>
+      <c r="J14" s="37"/>
     </row>
     <row r="15" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C15" s="18" t="s">
@@ -1544,11 +1544,11 @@
       <c r="H15" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="I15" s="53"/>
+      <c r="I15" s="42"/>
       <c r="J15" s="21"/>
     </row>
     <row r="16" spans="3:10" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="C16" s="37" t="s">
+      <c r="C16" s="51" t="s">
         <v>28</v>
       </c>
       <c r="D16" s="29" t="s">
@@ -1561,14 +1561,14 @@
         <v>46050</v>
       </c>
       <c r="G16" s="16">
-        <v>46051</v>
+        <v>46052</v>
       </c>
       <c r="H16" s="15"/>
-      <c r="I16" s="54"/>
+      <c r="I16" s="43"/>
       <c r="J16" s="17"/>
     </row>
     <row r="17" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C17" s="37"/>
+      <c r="C17" s="51"/>
       <c r="D17" s="28" t="s">
         <v>36</v>
       </c>
@@ -1579,16 +1579,16 @@
         <v>46050</v>
       </c>
       <c r="G17" s="6">
-        <v>46052</v>
+        <v>46054</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I17" s="51"/>
+      <c r="I17" s="40"/>
       <c r="J17" s="11"/>
     </row>
     <row r="18" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C18" s="37"/>
+      <c r="C18" s="51"/>
       <c r="D18" s="28" t="s">
         <v>57</v>
       </c>
@@ -1600,11 +1600,11 @@
         <v>46053</v>
       </c>
       <c r="H18" s="5"/>
-      <c r="I18" s="51"/>
+      <c r="I18" s="40"/>
       <c r="J18" s="11"/>
     </row>
     <row r="19" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C19" s="38"/>
+      <c r="C19" s="52"/>
       <c r="D19" s="5" t="s">
         <v>37</v>
       </c>
@@ -1613,14 +1613,14 @@
         <v>46050</v>
       </c>
       <c r="G19" s="6">
-        <v>46053</v>
+        <v>46055</v>
       </c>
       <c r="H19" s="5"/>
-      <c r="I19" s="51"/>
+      <c r="I19" s="40"/>
       <c r="J19" s="11"/>
     </row>
     <row r="20" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C20" s="39" t="s">
+      <c r="C20" s="53" t="s">
         <v>29</v>
       </c>
       <c r="D20" s="27" t="s">
@@ -1633,14 +1633,14 @@
         <v>46050</v>
       </c>
       <c r="G20" s="16">
-        <v>46051</v>
+        <v>46052</v>
       </c>
       <c r="H20" s="5"/>
-      <c r="I20" s="51"/>
+      <c r="I20" s="40"/>
       <c r="J20" s="11"/>
     </row>
     <row r="21" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C21" s="37"/>
+      <c r="C21" s="51"/>
       <c r="D21" s="28" t="s">
         <v>38</v>
       </c>
@@ -1651,14 +1651,14 @@
         <v>46050</v>
       </c>
       <c r="G21" s="6">
-        <v>46052</v>
+        <v>46054</v>
       </c>
       <c r="H21" s="5"/>
-      <c r="I21" s="51"/>
+      <c r="I21" s="40"/>
       <c r="J21" s="11"/>
     </row>
     <row r="22" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C22" s="37"/>
+      <c r="C22" s="51"/>
       <c r="D22" s="28" t="s">
         <v>57</v>
       </c>
@@ -1670,11 +1670,11 @@
         <v>46053</v>
       </c>
       <c r="H22" s="5"/>
-      <c r="I22" s="51"/>
+      <c r="I22" s="40"/>
       <c r="J22" s="11"/>
     </row>
     <row r="23" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C23" s="38"/>
+      <c r="C23" s="52"/>
       <c r="D23" s="5" t="s">
         <v>37</v>
       </c>
@@ -1683,14 +1683,14 @@
         <v>46050</v>
       </c>
       <c r="G23" s="6">
-        <v>46053</v>
+        <v>46055</v>
       </c>
       <c r="H23" s="5"/>
-      <c r="I23" s="51"/>
+      <c r="I23" s="40"/>
       <c r="J23" s="11"/>
     </row>
     <row r="24" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C24" s="39" t="s">
+      <c r="C24" s="53" t="s">
         <v>30</v>
       </c>
       <c r="D24" s="27" t="s">
@@ -1703,14 +1703,14 @@
         <v>46050</v>
       </c>
       <c r="G24" s="16">
-        <v>46051</v>
+        <v>46052</v>
       </c>
       <c r="H24" s="5"/>
-      <c r="I24" s="51"/>
+      <c r="I24" s="40"/>
       <c r="J24" s="11"/>
     </row>
     <row r="25" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C25" s="37"/>
+      <c r="C25" s="51"/>
       <c r="D25" s="28" t="s">
         <v>36</v>
       </c>
@@ -1721,14 +1721,14 @@
         <v>46050</v>
       </c>
       <c r="G25" s="6">
-        <v>46052</v>
+        <v>46054</v>
       </c>
       <c r="H25" s="5"/>
-      <c r="I25" s="51"/>
+      <c r="I25" s="40"/>
       <c r="J25" s="11"/>
     </row>
     <row r="26" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C26" s="37"/>
+      <c r="C26" s="51"/>
       <c r="D26" s="28" t="s">
         <v>57</v>
       </c>
@@ -1740,11 +1740,11 @@
         <v>46053</v>
       </c>
       <c r="H26" s="5"/>
-      <c r="I26" s="51"/>
+      <c r="I26" s="40"/>
       <c r="J26" s="11"/>
     </row>
     <row r="27" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C27" s="38"/>
+      <c r="C27" s="52"/>
       <c r="D27" s="5" t="s">
         <v>37</v>
       </c>
@@ -1753,14 +1753,14 @@
         <v>46050</v>
       </c>
       <c r="G27" s="6">
-        <v>46053</v>
+        <v>46055</v>
       </c>
       <c r="H27" s="5"/>
-      <c r="I27" s="51"/>
+      <c r="I27" s="40"/>
       <c r="J27" s="11"/>
     </row>
     <row r="28" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C28" s="39" t="s">
+      <c r="C28" s="53" t="s">
         <v>31</v>
       </c>
       <c r="D28" s="27" t="s">
@@ -1773,14 +1773,14 @@
         <v>46050</v>
       </c>
       <c r="G28" s="16">
-        <v>46051</v>
+        <v>46052</v>
       </c>
       <c r="H28" s="5"/>
-      <c r="I28" s="51"/>
+      <c r="I28" s="40"/>
       <c r="J28" s="11"/>
     </row>
     <row r="29" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C29" s="37"/>
+      <c r="C29" s="51"/>
       <c r="D29" s="28" t="s">
         <v>36</v>
       </c>
@@ -1791,14 +1791,14 @@
         <v>46050</v>
       </c>
       <c r="G29" s="6">
-        <v>46052</v>
+        <v>46054</v>
       </c>
       <c r="H29" s="5"/>
-      <c r="I29" s="51"/>
+      <c r="I29" s="40"/>
       <c r="J29" s="11"/>
     </row>
     <row r="30" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C30" s="37"/>
+      <c r="C30" s="51"/>
       <c r="D30" s="28" t="s">
         <v>57</v>
       </c>
@@ -1810,11 +1810,11 @@
         <v>46053</v>
       </c>
       <c r="H30" s="5"/>
-      <c r="I30" s="51"/>
+      <c r="I30" s="40"/>
       <c r="J30" s="11"/>
     </row>
     <row r="31" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C31" s="38"/>
+      <c r="C31" s="52"/>
       <c r="D31" s="5" t="s">
         <v>37</v>
       </c>
@@ -1823,14 +1823,14 @@
         <v>46050</v>
       </c>
       <c r="G31" s="6">
-        <v>46053</v>
+        <v>46055</v>
       </c>
       <c r="H31" s="5"/>
-      <c r="I31" s="51"/>
+      <c r="I31" s="40"/>
       <c r="J31" s="11"/>
     </row>
     <row r="32" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C32" s="39" t="s">
+      <c r="C32" s="53" t="s">
         <v>32</v>
       </c>
       <c r="D32" s="27" t="s">
@@ -1843,14 +1843,14 @@
         <v>46050</v>
       </c>
       <c r="G32" s="16">
-        <v>46051</v>
+        <v>46052</v>
       </c>
       <c r="H32" s="5"/>
-      <c r="I32" s="51"/>
+      <c r="I32" s="40"/>
       <c r="J32" s="11"/>
     </row>
     <row r="33" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C33" s="37"/>
+      <c r="C33" s="51"/>
       <c r="D33" s="28" t="s">
         <v>36</v>
       </c>
@@ -1861,14 +1861,14 @@
         <v>46050</v>
       </c>
       <c r="G33" s="6">
-        <v>46052</v>
+        <v>46054</v>
       </c>
       <c r="H33" s="5"/>
-      <c r="I33" s="51"/>
+      <c r="I33" s="40"/>
       <c r="J33" s="11"/>
     </row>
     <row r="34" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C34" s="37"/>
+      <c r="C34" s="51"/>
       <c r="D34" s="28" t="s">
         <v>57</v>
       </c>
@@ -1880,11 +1880,11 @@
         <v>46053</v>
       </c>
       <c r="H34" s="5"/>
-      <c r="I34" s="51"/>
+      <c r="I34" s="40"/>
       <c r="J34" s="11"/>
     </row>
     <row r="35" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C35" s="38"/>
+      <c r="C35" s="52"/>
       <c r="D35" s="5" t="s">
         <v>37</v>
       </c>
@@ -1895,14 +1895,14 @@
         <v>46050</v>
       </c>
       <c r="G35" s="6">
-        <v>46053</v>
+        <v>46055</v>
       </c>
       <c r="H35" s="5"/>
-      <c r="I35" s="51"/>
+      <c r="I35" s="40"/>
       <c r="J35" s="11"/>
     </row>
     <row r="36" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C36" s="32" t="s">
+      <c r="C36" s="46" t="s">
         <v>33</v>
       </c>
       <c r="D36" s="5" t="s">
@@ -1915,14 +1915,14 @@
         <v>46050</v>
       </c>
       <c r="G36" s="6">
-        <v>46053</v>
+        <v>46055</v>
       </c>
       <c r="H36" s="5"/>
-      <c r="I36" s="51"/>
+      <c r="I36" s="40"/>
       <c r="J36" s="11"/>
     </row>
     <row r="37" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C37" s="33"/>
+      <c r="C37" s="47"/>
       <c r="D37" s="5" t="s">
         <v>56</v>
       </c>
@@ -1933,42 +1933,40 @@
         <v>46050</v>
       </c>
       <c r="G37" s="6">
-        <v>46054</v>
+        <v>46056</v>
       </c>
       <c r="H37" s="5"/>
-      <c r="I37" s="51"/>
+      <c r="I37" s="40"/>
       <c r="J37" s="11"/>
     </row>
     <row r="38" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C38" s="33"/>
+      <c r="C38" s="47"/>
       <c r="D38" s="28" t="s">
         <v>57</v>
       </c>
       <c r="E38" s="26"/>
       <c r="F38" s="16"/>
-      <c r="G38" s="6">
-        <v>46053</v>
-      </c>
+      <c r="G38" s="6"/>
       <c r="H38" s="5"/>
-      <c r="I38" s="51"/>
+      <c r="I38" s="40"/>
       <c r="J38" s="11"/>
     </row>
     <row r="39" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C39" s="34"/>
+      <c r="C39" s="48"/>
       <c r="D39" s="5" t="s">
         <v>61</v>
       </c>
       <c r="E39" s="26" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F39" s="16">
         <v>46050</v>
       </c>
       <c r="G39" s="6">
-        <v>46054</v>
+        <v>46057</v>
       </c>
       <c r="H39" s="5"/>
-      <c r="I39" s="51"/>
+      <c r="I39" s="40"/>
       <c r="J39" s="11"/>
     </row>
     <row r="40" spans="3:10" x14ac:dyDescent="0.35">
@@ -1981,10 +1979,10 @@
       <c r="E40" s="26"/>
       <c r="F40" s="16"/>
       <c r="G40" s="6">
-        <v>46054</v>
+        <v>46057</v>
       </c>
       <c r="H40" s="5"/>
-      <c r="I40" s="51"/>
+      <c r="I40" s="40"/>
       <c r="J40" s="11"/>
     </row>
     <row r="41" spans="3:10" x14ac:dyDescent="0.35">
@@ -2002,7 +2000,7 @@
         <v>46055</v>
       </c>
       <c r="H41" s="5"/>
-      <c r="I41" s="51"/>
+      <c r="I41" s="40"/>
       <c r="J41" s="11"/>
     </row>
     <row r="42" spans="3:10" x14ac:dyDescent="0.35">
@@ -2017,10 +2015,10 @@
       </c>
       <c r="F42" s="6"/>
       <c r="G42" s="6">
-        <v>46053</v>
+        <v>46055</v>
       </c>
       <c r="H42" s="5"/>
-      <c r="I42" s="51"/>
+      <c r="I42" s="40"/>
       <c r="J42" s="11"/>
     </row>
     <row r="43" spans="3:10" x14ac:dyDescent="0.35">
@@ -2033,10 +2031,10 @@
       </c>
       <c r="F43" s="6"/>
       <c r="G43" s="6">
-        <v>46053</v>
+        <v>46055</v>
       </c>
       <c r="H43" s="5"/>
-      <c r="I43" s="51"/>
+      <c r="I43" s="40"/>
       <c r="J43" s="11"/>
     </row>
     <row r="44" spans="3:10" ht="72.5" x14ac:dyDescent="0.35">
@@ -2048,7 +2046,7 @@
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
       <c r="H44" s="5"/>
-      <c r="I44" s="51"/>
+      <c r="I44" s="40"/>
       <c r="J44" s="11"/>
     </row>
     <row r="45" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2058,7 +2056,7 @@
       <c r="F45" s="14"/>
       <c r="G45" s="14"/>
       <c r="H45" s="12"/>
-      <c r="I45" s="55"/>
+      <c r="I45" s="44"/>
       <c r="J45" s="13"/>
     </row>
     <row r="46" spans="3:10" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Current File 29 Jan 2026
Updated in the comments log today's progress. Given color code to status column. Added task for retrospective review.
</commit_message>
<xml_diff>
--- a/meetings/standups/Product Backlog Project Network Security Analysis Cloud Network.xlsx
+++ b/meetings/standups/Product Backlog Project Network Security Analysis Cloud Network.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="202300"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{415450CB-5CC5-4113-A6E5-BAF9D5F97AA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25219FF2-191D-46B2-9F55-D20B1C4E2016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{D772D2C9-32D6-40F8-B3B7-1BC774CEBB4D}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="75">
   <si>
     <t>Assigned  to</t>
   </si>
@@ -62,9 +62,6 @@
   </si>
   <si>
     <t>Date Of Completion</t>
-  </si>
-  <si>
-    <t>Yes</t>
   </si>
   <si>
     <t>NA</t>
@@ -262,9 +259,6 @@
     <t>Status Change Comment Log</t>
   </si>
   <si>
-    <t>28-01: Due meeting notes issue in place of original google meets, Zoom is decided to be used</t>
-  </si>
-  <si>
     <t>28-01 All other members confirmed</t>
   </si>
   <si>
@@ -272,6 +266,36 @@
   </si>
   <si>
     <t>Setting up Sprint Time line and Sprint Backlog Doc</t>
+  </si>
+  <si>
+    <t>28-01: Due meeting notes issue in place of original google meets, Zoom is decided to be used. Ojas Created daily zoom link</t>
+  </si>
+  <si>
+    <t>To be assigned</t>
+  </si>
+  <si>
+    <t>29/02/2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29-01: Nigam confirmed AI research - part over </t>
+  </si>
+  <si>
+    <t>29-01: Nigam is starting now the report part</t>
+  </si>
+  <si>
+    <t>29-01 Nigam prompts are ready.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29-01 Sachin has requested the exentsion till 4th. Yet to get confirmation </t>
+  </si>
+  <si>
+    <t>Retrospective review</t>
+  </si>
+  <si>
+    <t>29-01 Sachin added the task to backlog</t>
+  </si>
+  <si>
+    <t>29-01 Sachin has identified few prompts, completed AI research,building the outline now.</t>
   </si>
 </sst>
 </file>
@@ -928,7 +952,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="4">
     <dxf>
       <font>
         <b/>
@@ -938,6 +962,40 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1273,10 +1331,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20F47E7B-76B1-4927-897A-8DA0F75CCE1B}">
   <dimension ref="C2:J53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <pane ySplit="12" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <pane ySplit="12" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B2" sqref="B2"/>
-      <selection pane="bottomLeft" activeCell="J41" sqref="J41"/>
+      <selection pane="bottomLeft" activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1294,10 +1352,10 @@
   <sheetData>
     <row r="2" spans="3:10" ht="17" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C2" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" s="49" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E2" s="50"/>
       <c r="F2" s="50"/>
@@ -1305,27 +1363,27 @@
     </row>
     <row r="3" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="E3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="4" spans="3:10" ht="29" x14ac:dyDescent="0.35">
       <c r="C4" s="32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>3</v>
@@ -1339,10 +1397,10 @@
     </row>
     <row r="5" spans="3:10" ht="32" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C5" s="32" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>2</v>
@@ -1350,10 +1408,10 @@
     </row>
     <row r="6" spans="3:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C6" s="32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>8</v>
@@ -1370,16 +1428,16 @@
         <v>0</v>
       </c>
       <c r="F7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="8" t="s">
-        <v>13</v>
-      </c>
       <c r="H7" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I7" s="39" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J7" s="9" t="s">
         <v>9</v>
@@ -1398,10 +1456,10 @@
         <v>46050</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I8" s="40" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J8" s="11">
         <v>46043</v>
@@ -1410,7 +1468,7 @@
     <row r="9" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C9" s="55"/>
       <c r="D9" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>2</v>
@@ -1420,7 +1478,7 @@
         <v>46050</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I9" s="40"/>
       <c r="J9" s="11">
@@ -1430,7 +1488,7 @@
     <row r="10" spans="3:10" ht="29" x14ac:dyDescent="0.35">
       <c r="C10" s="56"/>
       <c r="D10" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>8</v>
@@ -1440,10 +1498,10 @@
         <v>46050</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I10" s="40" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J10" s="11">
         <v>46043</v>
@@ -1451,10 +1509,10 @@
     </row>
     <row r="11" spans="3:10" ht="29" x14ac:dyDescent="0.35">
       <c r="C11" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>21</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>22</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>2</v>
@@ -1464,16 +1522,16 @@
         <v>46055</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I11" s="40" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J11" s="11"/>
     </row>
-    <row r="12" spans="3:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="12" spans="3:10" ht="72.5" x14ac:dyDescent="0.35">
       <c r="C12" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5" t="s">
@@ -1484,18 +1542,18 @@
         <v>46081</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I12" s="40" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J12" s="11">
-        <v>46047</v>
-      </c>
-    </row>
-    <row r="13" spans="3:10" ht="29" x14ac:dyDescent="0.35">
+        <v>46050</v>
+      </c>
+    </row>
+    <row r="13" spans="3:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C13" s="45" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="5" t="s">
@@ -1505,16 +1563,20 @@
       <c r="G13" s="6">
         <v>46051</v>
       </c>
-      <c r="H13" s="5"/>
-      <c r="I13" s="40"/>
+      <c r="H13" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="I13" s="40" t="s">
+        <v>71</v>
+      </c>
       <c r="J13" s="11"/>
     </row>
     <row r="14" spans="3:10" ht="29" x14ac:dyDescent="0.35">
       <c r="C14" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="38" t="s">
         <v>54</v>
-      </c>
-      <c r="D14" s="38" t="s">
-        <v>55</v>
       </c>
       <c r="E14" s="35" t="s">
         <v>3</v>
@@ -1524,14 +1586,14 @@
         <v>46051</v>
       </c>
       <c r="H14" s="35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I14" s="41"/>
       <c r="J14" s="37"/>
     </row>
     <row r="15" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C15" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D15" s="19"/>
       <c r="E15" s="19"/>
@@ -1542,17 +1604,17 @@
         <v>46051</v>
       </c>
       <c r="H15" s="19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I15" s="42"/>
       <c r="J15" s="21"/>
     </row>
     <row r="16" spans="3:10" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="C16" s="51" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E16" s="25" t="s">
         <v>2</v>
@@ -1563,14 +1625,16 @@
       <c r="G16" s="16">
         <v>46052</v>
       </c>
-      <c r="H16" s="15"/>
+      <c r="H16" s="15" t="s">
+        <v>48</v>
+      </c>
       <c r="I16" s="43"/>
       <c r="J16" s="17"/>
     </row>
     <row r="17" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C17" s="51"/>
       <c r="D17" s="28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E17" s="25" t="s">
         <v>2</v>
@@ -1582,7 +1646,7 @@
         <v>46054</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="I17" s="40"/>
       <c r="J17" s="11"/>
@@ -1590,7 +1654,7 @@
     <row r="18" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C18" s="51"/>
       <c r="D18" s="28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E18" s="25" t="s">
         <v>2</v>
@@ -1599,14 +1663,16 @@
       <c r="G18" s="6">
         <v>46053</v>
       </c>
-      <c r="H18" s="5"/>
+      <c r="H18" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="I18" s="40"/>
       <c r="J18" s="11"/>
     </row>
     <row r="19" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C19" s="52"/>
       <c r="D19" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E19" s="26"/>
       <c r="F19" s="16">
@@ -1615,16 +1681,18 @@
       <c r="G19" s="6">
         <v>46055</v>
       </c>
-      <c r="H19" s="5"/>
+      <c r="H19" s="5" t="s">
+        <v>66</v>
+      </c>
       <c r="I19" s="40"/>
       <c r="J19" s="11"/>
     </row>
     <row r="20" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C20" s="53" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D20" s="27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E20" s="26" t="s">
         <v>3</v>
@@ -1635,14 +1703,16 @@
       <c r="G20" s="16">
         <v>46052</v>
       </c>
-      <c r="H20" s="5"/>
+      <c r="H20" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="I20" s="40"/>
       <c r="J20" s="11"/>
     </row>
     <row r="21" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C21" s="51"/>
       <c r="D21" s="28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E21" s="26" t="s">
         <v>3</v>
@@ -1653,14 +1723,16 @@
       <c r="G21" s="6">
         <v>46054</v>
       </c>
-      <c r="H21" s="5"/>
+      <c r="H21" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="I21" s="40"/>
       <c r="J21" s="11"/>
     </row>
     <row r="22" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C22" s="51"/>
       <c r="D22" s="28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E22" s="26" t="s">
         <v>3</v>
@@ -1669,14 +1741,16 @@
       <c r="G22" s="6">
         <v>46053</v>
       </c>
-      <c r="H22" s="5"/>
+      <c r="H22" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="I22" s="40"/>
       <c r="J22" s="11"/>
     </row>
     <row r="23" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C23" s="52"/>
       <c r="D23" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E23" s="26"/>
       <c r="F23" s="16">
@@ -1685,16 +1759,18 @@
       <c r="G23" s="6">
         <v>46055</v>
       </c>
-      <c r="H23" s="5"/>
+      <c r="H23" s="5" t="s">
+        <v>66</v>
+      </c>
       <c r="I23" s="40"/>
       <c r="J23" s="11"/>
     </row>
-    <row r="24" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:10" ht="29" x14ac:dyDescent="0.35">
       <c r="C24" s="53" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D24" s="27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E24" s="26" t="s">
         <v>4</v>
@@ -1705,14 +1781,20 @@
       <c r="G24" s="16">
         <v>46052</v>
       </c>
-      <c r="H24" s="5"/>
-      <c r="I24" s="40"/>
-      <c r="J24" s="11"/>
-    </row>
-    <row r="25" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="H24" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="I24" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="J24" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="3:10" ht="29" x14ac:dyDescent="0.25">
       <c r="C25" s="51"/>
       <c r="D25" s="28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E25" s="26" t="s">
         <v>4</v>
@@ -1723,14 +1805,18 @@
       <c r="G25" s="6">
         <v>46054</v>
       </c>
-      <c r="H25" s="5"/>
-      <c r="I25" s="40"/>
+      <c r="H25" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="I25" s="40" t="s">
+        <v>69</v>
+      </c>
       <c r="J25" s="11"/>
     </row>
-    <row r="26" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:10" ht="29" x14ac:dyDescent="0.25">
       <c r="C26" s="51"/>
       <c r="D26" s="28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E26" s="26" t="s">
         <v>4</v>
@@ -1739,14 +1825,18 @@
       <c r="G26" s="6">
         <v>46053</v>
       </c>
-      <c r="H26" s="5"/>
-      <c r="I26" s="40"/>
+      <c r="H26" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="I26" s="40" t="s">
+        <v>70</v>
+      </c>
       <c r="J26" s="11"/>
     </row>
     <row r="27" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C27" s="52"/>
       <c r="D27" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E27" s="26"/>
       <c r="F27" s="16">
@@ -1755,16 +1845,18 @@
       <c r="G27" s="6">
         <v>46055</v>
       </c>
-      <c r="H27" s="5"/>
+      <c r="H27" s="5" t="s">
+        <v>66</v>
+      </c>
       <c r="I27" s="40"/>
       <c r="J27" s="11"/>
     </row>
-    <row r="28" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:10" ht="58" x14ac:dyDescent="0.35">
       <c r="C28" s="53" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D28" s="27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E28" s="26" t="s">
         <v>5</v>
@@ -1775,14 +1867,18 @@
       <c r="G28" s="16">
         <v>46052</v>
       </c>
-      <c r="H28" s="5"/>
-      <c r="I28" s="40"/>
+      <c r="H28" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="I28" s="40" t="s">
+        <v>74</v>
+      </c>
       <c r="J28" s="11"/>
     </row>
     <row r="29" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C29" s="51"/>
       <c r="D29" s="28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E29" s="26" t="s">
         <v>5</v>
@@ -1793,14 +1889,16 @@
       <c r="G29" s="6">
         <v>46054</v>
       </c>
-      <c r="H29" s="5"/>
+      <c r="H29" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="I29" s="40"/>
       <c r="J29" s="11"/>
     </row>
     <row r="30" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C30" s="51"/>
       <c r="D30" s="28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E30" s="26" t="s">
         <v>5</v>
@@ -1809,14 +1907,16 @@
       <c r="G30" s="6">
         <v>46053</v>
       </c>
-      <c r="H30" s="5"/>
+      <c r="H30" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="I30" s="40"/>
       <c r="J30" s="11"/>
     </row>
     <row r="31" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C31" s="52"/>
       <c r="D31" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E31" s="26"/>
       <c r="F31" s="16">
@@ -1825,16 +1925,18 @@
       <c r="G31" s="6">
         <v>46055</v>
       </c>
-      <c r="H31" s="5"/>
+      <c r="H31" s="5" t="s">
+        <v>66</v>
+      </c>
       <c r="I31" s="40"/>
       <c r="J31" s="11"/>
     </row>
     <row r="32" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C32" s="53" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D32" s="27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E32" s="26" t="s">
         <v>8</v>
@@ -1845,14 +1947,16 @@
       <c r="G32" s="16">
         <v>46052</v>
       </c>
-      <c r="H32" s="5"/>
+      <c r="H32" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="I32" s="40"/>
       <c r="J32" s="11"/>
     </row>
     <row r="33" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C33" s="51"/>
       <c r="D33" s="28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E33" s="26" t="s">
         <v>8</v>
@@ -1863,14 +1967,16 @@
       <c r="G33" s="6">
         <v>46054</v>
       </c>
-      <c r="H33" s="5"/>
+      <c r="H33" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="I33" s="40"/>
       <c r="J33" s="11"/>
     </row>
     <row r="34" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C34" s="51"/>
       <c r="D34" s="28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E34" s="26" t="s">
         <v>5</v>
@@ -1879,14 +1985,16 @@
       <c r="G34" s="6">
         <v>46053</v>
       </c>
-      <c r="H34" s="5"/>
+      <c r="H34" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="I34" s="40"/>
       <c r="J34" s="11"/>
     </row>
     <row r="35" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C35" s="52"/>
       <c r="D35" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E35" s="26" t="s">
         <v>8</v>
@@ -1897,16 +2005,18 @@
       <c r="G35" s="6">
         <v>46055</v>
       </c>
-      <c r="H35" s="5"/>
+      <c r="H35" s="5" t="s">
+        <v>66</v>
+      </c>
       <c r="I35" s="40"/>
       <c r="J35" s="11"/>
     </row>
     <row r="36" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C36" s="46" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E36" s="26" t="s">
         <v>5</v>
@@ -1917,14 +2027,16 @@
       <c r="G36" s="6">
         <v>46055</v>
       </c>
-      <c r="H36" s="5"/>
+      <c r="H36" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="I36" s="40"/>
       <c r="J36" s="11"/>
     </row>
     <row r="37" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C37" s="47"/>
       <c r="D37" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E37" s="26" t="s">
         <v>8</v>
@@ -1935,26 +2047,30 @@
       <c r="G37" s="6">
         <v>46056</v>
       </c>
-      <c r="H37" s="5"/>
+      <c r="H37" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="I37" s="40"/>
       <c r="J37" s="11"/>
     </row>
     <row r="38" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C38" s="47"/>
       <c r="D38" s="28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E38" s="26"/>
       <c r="F38" s="16"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="5"/>
+      <c r="H38" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="I38" s="40"/>
       <c r="J38" s="11"/>
     </row>
     <row r="39" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C39" s="48"/>
       <c r="D39" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E39" s="26" t="s">
         <v>3</v>
@@ -1965,30 +2081,34 @@
       <c r="G39" s="6">
         <v>46057</v>
       </c>
-      <c r="H39" s="5"/>
+      <c r="H39" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="I39" s="40"/>
       <c r="J39" s="11"/>
     </row>
     <row r="40" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C40" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D40" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>59</v>
       </c>
       <c r="E40" s="26"/>
       <c r="F40" s="16"/>
       <c r="G40" s="6">
         <v>46057</v>
       </c>
-      <c r="H40" s="5"/>
+      <c r="H40" s="5" t="s">
+        <v>66</v>
+      </c>
       <c r="I40" s="40"/>
       <c r="J40" s="11"/>
     </row>
     <row r="41" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C41" s="22"/>
       <c r="D41" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E41" s="26" t="s">
         <v>8</v>
@@ -1999,47 +2119,53 @@
       <c r="G41" s="6">
         <v>46055</v>
       </c>
-      <c r="H41" s="5"/>
+      <c r="H41" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="I41" s="40"/>
       <c r="J41" s="11"/>
     </row>
     <row r="42" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C42" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="D42" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="E42" s="26" t="s">
         <v>2</v>
       </c>
       <c r="F42" s="6"/>
       <c r="G42" s="6">
-        <v>46055</v>
-      </c>
-      <c r="H42" s="5"/>
+        <v>46057</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="I42" s="40"/>
       <c r="J42" s="11"/>
     </row>
     <row r="43" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C43" s="24"/>
       <c r="D43" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E43" s="26" t="s">
         <v>8</v>
       </c>
       <c r="F43" s="6"/>
       <c r="G43" s="6">
-        <v>46055</v>
-      </c>
-      <c r="H43" s="5"/>
+        <v>46057</v>
+      </c>
+      <c r="H43" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="I43" s="40"/>
       <c r="J43" s="11"/>
     </row>
     <row r="44" spans="3:10" ht="72.5" x14ac:dyDescent="0.35">
       <c r="C44" s="30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D44" s="5"/>
       <c r="E44" s="26"/>
@@ -2049,14 +2175,26 @@
       <c r="I44" s="40"/>
       <c r="J44" s="11"/>
     </row>
-    <row r="45" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C45" s="31"/>
+    <row r="45" spans="3:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C45" s="31" t="s">
+        <v>72</v>
+      </c>
       <c r="D45" s="12"/>
-      <c r="E45" s="12"/>
-      <c r="F45" s="14"/>
-      <c r="G45" s="14"/>
-      <c r="H45" s="12"/>
-      <c r="I45" s="44"/>
+      <c r="E45" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F45" s="14">
+        <v>46051</v>
+      </c>
+      <c r="G45" s="14">
+        <v>46058</v>
+      </c>
+      <c r="H45" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="I45" s="44" t="s">
+        <v>73</v>
+      </c>
       <c r="J45" s="13"/>
     </row>
     <row r="46" spans="3:10" x14ac:dyDescent="0.35">
@@ -2094,8 +2232,19 @@
     <mergeCell ref="C32:C35"/>
     <mergeCell ref="C8:C10"/>
   </mergeCells>
+  <conditionalFormatting sqref="H8:H45">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="assign">
+      <formula>NOT(ISERROR(SEARCH("assign",H8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="To Do">
+      <formula>NOT(ISERROR(SEARCH("To Do",H8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="progress">
+      <formula>NOT(ISERROR(SEARCH("progress",H8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="H8:I47">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",H8)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2103,7 +2252,7 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{96206D46-0350-46DE-AF9C-49F24259762A}">
           <x14:formula1>
             <xm:f>Sheet2!$C$3:$C$9</xm:f>
@@ -2114,13 +2263,19 @@
           <x14:formula1>
             <xm:f>Sheet2!$E$3:$E$6</xm:f>
           </x14:formula1>
-          <xm:sqref>I46:I76 H8:H76</xm:sqref>
+          <xm:sqref>I46:I76 H8:H12 H46:H76</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3E1289D9-77B0-49DF-AB7D-886206063157}">
           <x14:formula1>
             <xm:f>Sheet2!$C$3:$C$7</xm:f>
           </x14:formula1>
           <xm:sqref>E4:E6</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{58D95D59-36A4-4F0E-B0A8-FF8EB27CDB5D}">
+          <x14:formula1>
+            <xm:f>Sheet2!$E$3:$E$8</xm:f>
+          </x14:formula1>
+          <xm:sqref>H13:H45</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2130,10 +2285,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{259E51CE-4FCE-4CDE-B1F0-7C20793B2EB7}">
-  <dimension ref="C3:E7"/>
+  <dimension ref="C3:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2143,7 +2298,7 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="3:5" x14ac:dyDescent="0.35">
@@ -2151,7 +2306,7 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.35">
@@ -2159,7 +2314,7 @@
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="3:5" x14ac:dyDescent="0.35">
@@ -2167,7 +2322,7 @@
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="3:5" x14ac:dyDescent="0.35">
@@ -2175,7 +2330,12 @@
         <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>11</v>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="E8" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>